<commit_message>
Adding classification and clustering models
</commit_message>
<xml_diff>
--- a/Employees.xlsx
+++ b/Employees.xlsx
@@ -1,29 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\00-MLSamples\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yousif Ennwa\Desktop\Data_Analysis\ML-Samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D6498D8-95E3-43D7-95C3-512BA583A8E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="4"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NewEmployees" sheetId="3" r:id="rId1"/>
     <sheet name="Employees" sheetId="2" r:id="rId2"/>
     <sheet name="Sales" sheetId="4" r:id="rId3"/>
     <sheet name="ConcatenatedSheet" sheetId="1" r:id="rId4"/>
-    <sheet name="Names" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="9">
   <si>
     <t>Salary</t>
   </si>
@@ -51,45 +51,12 @@
   <si>
     <t>Year</t>
   </si>
-  <si>
-    <t>Sentence</t>
-  </si>
-  <si>
-    <t>Class</t>
-  </si>
-  <si>
-    <t>Hello</t>
-  </si>
-  <si>
-    <t>Ahmed</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Mohamed</t>
-  </si>
-  <si>
-    <t>Verb</t>
-  </si>
-  <si>
-    <t>Welcome</t>
-  </si>
-  <si>
-    <t>Come</t>
-  </si>
-  <si>
-    <t>Tell</t>
-  </si>
-  <si>
-    <t>Salah</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -110,13 +77,6 @@
       <color rgb="FF000000"/>
       <name val="Courier New"/>
       <family val="3"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -154,7 +114,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -162,7 +122,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -256,6 +215,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -291,6 +267,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -466,7 +459,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -793,7 +786,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1120,7 +1113,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1331,10 +1324,10 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1887,88 +1880,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B8"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="14.140625" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>